<commit_message>
Add data in database
</commit_message>
<xml_diff>
--- a/other/Diagrammes.xlsx
+++ b/other/Diagrammes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\garage\other\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA7B8BB-D843-4BE1-AF19-D06759A44454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C970BBB-F4BA-403B-B486-38E4FF991F85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="110">
   <si>
     <t>&lt;&lt;include&gt;&gt;</t>
   </si>
@@ -272,9 +272,6 @@
     <t xml:space="preserve"> - day : string</t>
   </si>
   <si>
-    <t xml:space="preserve"> - hours : time</t>
-  </si>
-  <si>
     <t xml:space="preserve"> - rating : int</t>
   </si>
   <si>
@@ -332,12 +329,6 @@
     <t>Models</t>
   </si>
   <si>
-    <t xml:space="preserve"> - has_equipment : int</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> - has_option : int</t>
-  </si>
-  <si>
     <t>0*             has</t>
   </si>
   <si>
@@ -369,6 +360,15 @@
   </si>
   <si>
     <t xml:space="preserve"> - has_brand : string</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - hours : string</t>
+  </si>
+  <si>
+    <t xml:space="preserve">      1*</t>
+  </si>
+  <si>
+    <t xml:space="preserve">        1</t>
   </si>
 </sst>
 </file>
@@ -541,8 +541,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -9381,13 +9381,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9431,13 +9431,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>27214</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>176893</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -9481,13 +9481,13 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>830036</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>68037</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>1306286</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>87764</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -9806,15 +9806,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>27215</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:colOff>68036</xdr:colOff>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>13606</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>81643</xdr:rowOff>
+      <xdr:rowOff>13607</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -9829,8 +9829,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8436429" y="4762500"/>
-          <a:ext cx="1537606" cy="81643"/>
+          <a:off x="8477250" y="4191000"/>
+          <a:ext cx="1496785" cy="585107"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -10201,6 +10201,116 @@
         <a:solidFill>
           <a:schemeClr val="bg1"/>
         </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="fr-FR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>625928</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>27214</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>625928</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Connecteur droit 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2344244D-56AC-42CD-B9A1-F3F20A0022A5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11919857" y="4599214"/>
+          <a:ext cx="0" cy="734786"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>394606</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>149679</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>870856</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>169406</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Organigramme : Décision 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56DD2751-50BE-46EE-BD70-C40BE6DF93C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="11688535" y="5102679"/>
+          <a:ext cx="476250" cy="210227"/>
+        </a:xfrm>
+        <a:prstGeom prst="flowChartDecision">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -10986,7 +11096,7 @@
       </c>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="R7" s="1"/>
     </row>
@@ -11117,7 +11227,7 @@
   <dimension ref="A3:L47"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+      <selection activeCell="L38" sqref="L38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11157,13 +11267,13 @@
         <v>27</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G5" s="8" t="s">
         <v>26</v>
       </c>
       <c r="J5" s="14" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
@@ -11186,7 +11296,7 @@
       </c>
       <c r="G7" s="19"/>
       <c r="I7" s="13" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>26</v>
@@ -11218,7 +11328,7 @@
       <c r="E11" s="19"/>
       <c r="I11" s="13"/>
       <c r="J11" s="14" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.25">
@@ -11229,13 +11339,13 @@
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E13" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G13" s="14" t="s">
         <v>75</v>
       </c>
       <c r="I13" s="13" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="J13" s="8" t="s">
         <v>26</v>
@@ -11260,17 +11370,17 @@
         <v>76</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="G15" s="8" t="s">
-        <v>77</v>
+        <v>107</v>
       </c>
       <c r="J15" s="19"/>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B16" s="2"/>
       <c r="E16" s="15" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="F16" s="11">
         <v>1</v>
@@ -11291,6 +11401,7 @@
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="E18" s="19"/>
+      <c r="I18" s="13"/>
       <c r="J18"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
@@ -11298,21 +11409,20 @@
       <c r="B19" s="2"/>
       <c r="G19" s="13"/>
       <c r="H19" s="13"/>
-      <c r="I19" s="13"/>
-      <c r="J19"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="E20" s="14" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="G20" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H20" s="17"/>
-      <c r="I20" s="11"/>
-      <c r="J20"/>
+      <c r="J20" s="14" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
@@ -11324,8 +11434,9 @@
         <v>25</v>
       </c>
       <c r="H21" s="2"/>
-      <c r="I21" s="13"/>
-      <c r="J21"/>
+      <c r="J21" s="8" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
@@ -11334,9 +11445,15 @@
         <v>27</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H22" s="2"/>
+      <c r="I22" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="J22" s="8" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
@@ -11345,12 +11462,13 @@
         <v>28</v>
       </c>
       <c r="G23" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H23" s="2"/>
-      <c r="J23" s="14" t="s">
-        <v>96</v>
-      </c>
+      <c r="I23" s="11">
+        <v>1</v>
+      </c>
+      <c r="J23" s="9"/>
       <c r="L23" s="2"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -11360,90 +11478,82 @@
         <v>30</v>
       </c>
       <c r="F24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="G24" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H24" s="2"/>
-      <c r="J24" s="8" t="s">
-        <v>25</v>
-      </c>
+      <c r="J24" s="19"/>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E25" s="8" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F25">
         <v>1</v>
       </c>
       <c r="G25" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="H25" s="2"/>
-      <c r="I25" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="J25" s="8" t="s">
-        <v>26</v>
+      <c r="J25" s="12" t="s">
+        <v>108</v>
       </c>
       <c r="L25" s="17"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B26" s="17"/>
       <c r="E26" s="8" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G26" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H26" s="2"/>
-      <c r="I26" s="11">
-        <v>1</v>
-      </c>
-      <c r="J26" s="9"/>
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
       <c r="D27" s="13"/>
       <c r="E27" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="G27" s="21" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="G27" s="8" t="s">
+        <v>82</v>
       </c>
       <c r="H27" s="2"/>
-      <c r="J27" s="19"/>
       <c r="L27" s="2"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
       <c r="E28" s="8"/>
-      <c r="G28" s="15" t="s">
+      <c r="G28" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="2"/>
+      <c r="J28" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="H28" s="2"/>
-      <c r="J28"/>
       <c r="L28" s="2"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
       <c r="E29" s="19"/>
-      <c r="G29" s="15" t="s">
-        <v>102</v>
+      <c r="G29" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="H29" s="2"/>
       <c r="J29" s="14" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L29" s="2"/>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B30" s="2"/>
       <c r="E30" s="12"/>
-      <c r="G30" s="21" t="s">
-        <v>84</v>
+      <c r="G30" s="8" t="s">
+        <v>83</v>
       </c>
       <c r="H30" s="2"/>
       <c r="J30" s="8" t="s">
@@ -11453,14 +11563,14 @@
     <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B31" s="2"/>
       <c r="E31" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>93</v>
+        <v>103</v>
+      </c>
+      <c r="G31" s="8" t="s">
+        <v>92</v>
       </c>
       <c r="H31" s="2"/>
       <c r="I31" s="13" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="J31" s="8" t="s">
         <v>26</v>
@@ -11471,7 +11581,7 @@
         <v>25</v>
       </c>
       <c r="G32" s="15" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="H32" s="2"/>
       <c r="I32" s="11">
@@ -11485,7 +11595,7 @@
         <v>27</v>
       </c>
       <c r="G33" s="15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="H33" s="2"/>
       <c r="J33" s="9"/>
@@ -11518,7 +11628,7 @@
     <row r="37" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B37" s="2"/>
       <c r="E37" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I37" s="13"/>
     </row>
@@ -11529,7 +11639,7 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E39" s="10" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.25">
@@ -11569,6 +11679,9 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="J28" numberStoredAsText="1"/>
+  </ignoredErrors>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>